<commit_message>
* Transform email before compare
</commit_message>
<xml_diff>
--- a/src/test/resources/validate_doubts_test.xlsx
+++ b/src/test/resources/validate_doubts_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="116">
   <si>
     <t xml:space="preserve">Motivo duda</t>
   </si>
@@ -353,6 +353,21 @@
   </si>
   <si>
     <t xml:space="preserve">12º Curso Educación Primaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arroba con letras email no exacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pepitopalotes38@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pepito22 Palotes Pérez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altea22 Palotes Sánchez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pau8 Palotes Sánchez</t>
   </si>
 </sst>
 </file>
@@ -578,18 +593,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:Y24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="bottomLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.12"/>
@@ -1755,6 +1770,59 @@
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="6" t="n">
+        <v>777777777</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1782,6 +1850,8 @@
     <hyperlink ref="Q22" r:id="rId22" display="https://drive.google.com/open?id=1MepS_u_9h7_8AcPmbn0axFAzXK0aLDYR"/>
     <hyperlink ref="B23" r:id="rId23" display="pepitopalotes36@hotmail.com"/>
     <hyperlink ref="Q23" r:id="rId24" display="https://drive.google.com/open?id=1MepS_u_9h7_8AcPmbn0axFAzXK0aLDYR"/>
+    <hyperlink ref="B24" r:id="rId25" display="pepitopalotes38@hotmail.com"/>
+    <hyperlink ref="Q24" r:id="rId26" display="https://drive.google.com/open?id=1MepS_u_9h7_8AcPmbn0axFAzXK0aLDYR"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
* Finished with payed checks, tests and little refactor
</commit_message>
<xml_diff>
--- a/src/test/resources/validate_doubts_test.xlsx
+++ b/src/test/resources/validate_doubts_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="117">
   <si>
     <t xml:space="preserve">Motivo duda</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t xml:space="preserve">11º Curso Educación Primaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correcto</t>
   </si>
   <si>
     <t xml:space="preserve">pepitopalotes36@hotmail.com</t>
@@ -598,10 +601,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.77"/>
@@ -1721,12 +1724,14 @@
       <c r="Y22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9"/>
+      <c r="A23" s="9" t="s">
+        <v>106</v>
+      </c>
       <c r="B23" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D23" s="6" t="n">
         <v>777777777</v>
@@ -1739,7 +1744,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>17</v>
@@ -1750,10 +1755,10 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q23" s="7" t="s">
         <v>18</v>
@@ -1773,13 +1778,13 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D24" s="6" t="n">
         <v>777777777</v>
@@ -1792,7 +1797,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>17</v>
@@ -1803,7 +1808,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>105</v>

</xml_diff>